<commit_message>
integration tests for DSLOOKUP function are added. Tests are based on excel file with formula-expacted_value pattern
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Monthly_Data_Query_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Monthly_Data_Query_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="24150" windowHeight="11325"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="24150" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Formula</t>
   </si>
@@ -47,16 +47,19 @@
     <t>Company</t>
   </si>
   <si>
-    <t>Current_LT_Rating</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Corporate_Accounting_Regime</t>
+  </si>
+  <si>
+    <t>US GAAP</t>
+  </si>
+  <si>
+    <t>2012</t>
   </si>
 </sst>
 </file>
@@ -101,9 +104,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,12 +391,12 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.7109375" customWidth="1"/>
+    <col min="1" max="1" width="65.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -484,7 +488,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="e">
-        <f ca="1">DSLOOKUP("Monthly_Data_Query","Company","Alon USA Energy, Inc.","Year","2012","Current_LT_Rating","B2","Country")</f>
+        <f ca="1">DSLOOKUP("Monthly_Data_Query","Company","Alon USA Energy, Inc.","Year","2012","Corporate_Accounting_Regime","US GAAP","Country")</f>
         <v>#NAME?</v>
       </c>
       <c r="B9" t="s">
@@ -493,7 +497,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="e">
-        <f ca="1">DSLOOKUP("Monthly_Data_Query","Company","Alon USA Energy, Inc.","Current_LT_Rating","B2","Year","2012","Country")</f>
+        <f ca="1">DSLOOKUP("Monthly_Data_Query","Company","Alon USA Energy, Inc.","Corporate_Accounting_Regime","US GAAP","Year","2012","Country")</f>
         <v>#NAME?</v>
       </c>
       <c r="B10" t="s">
@@ -518,19 +522,19 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
         <v>7</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
         <v>8</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11">
-        <v>2012</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -544,7 +548,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="e">
-        <f ca="1">DSLOOKUP("Monthly_Data_Query","Secured_Debt", 0, "TOTAL_ASSETS", 1998193.287836, "Treasury_Stock_Issued_Repurchased")</f>
+        <f ca="1">DSLOOKUP("Monthly_Data_Query","Secured_Debt", 0, "GROSS_PROFIT", 4049115.256714, "Treasury_Stock_Issued_Repurchased")</f>
         <v>#NAME?</v>
       </c>
       <c r="B13">

</xml_diff>

<commit_message>
small cache for DsLookup is added
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Monthly_Data_Query_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Monthly_Data_Query_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4050" windowWidth="24150" windowHeight="11325"/>
+    <workbookView xWindow="0" yWindow="4500" windowWidth="24150" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>